<commit_message>
added characterisation tables and a function to aggregate private energy externalities
</commit_message>
<xml_diff>
--- a/classifications3.0.13_3_dec_2016.xlsx
+++ b/classifications3.0.13_3_dec_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" state="visible" r:id="rId2"/>
@@ -13947,22 +13947,22 @@
   </sheetPr>
   <dimension ref="B2:I150"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15893,16 +15893,17 @@
   </sheetPr>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16259,15 +16260,16 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16399,16 +16401,17 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16499,16 +16502,17 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16655,14 +16659,13 @@
   </sheetPr>
   <dimension ref="A1:C418"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="93.4132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="92.3367346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21281,15 +21284,16 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21382,18 +21386,18 @@
   </sheetPr>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E59" activeCellId="0" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="253" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22420,19 +22424,20 @@
   </sheetPr>
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26225,20 +26230,21 @@
   </sheetPr>
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31485,18 +31491,18 @@
   </sheetPr>
   <dimension ref="A1:E419"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.9897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37464,18 +37470,18 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37722,17 +37728,18 @@
   </sheetPr>
   <dimension ref="A1:E868"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.9132653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -50028,16 +50035,17 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>